<commit_message>
Fixes #1949 data importer parsing unit should be case insensitive
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Core.IntegrationTests/Data/Test5.xlsx
+++ b/tests/OSPSuite.Core.IntegrationTests/Data/Test5.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\OSPSuite.Core\tests\OSPSuite.Core.IntegrationTests\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2EA389-1898-42B9-A1E7-EA3D9C1165C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="12840" windowHeight="7995"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="33180" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,13 +33,13 @@
     <t>H</t>
   </si>
   <si>
-    <t>mg/l</t>
+    <t>mg/mL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +84,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -86,14 +92,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -131,9 +140,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +175,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,9 +227,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -376,14 +419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -440,24 +486,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes #1949 data importer parsing unit should be case insensitive (#1952)
* Fixes #1949 data importer parsing unit should be case insensitive

* Run resharper

* Remove fake to use real dimensions

* Remove fake to use real dimensions

* refactoring and removing further .HasUnit() calls

---------

Co-authored-by: georgeDaskalakis <37107428+georgeDaskalakis@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Core.IntegrationTests/Data/Test5.xlsx
+++ b/tests/OSPSuite.Core.IntegrationTests/Data/Test5.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\OSPSuite.Core\tests\OSPSuite.Core.IntegrationTests\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2EA389-1898-42B9-A1E7-EA3D9C1165C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="12840" windowHeight="7995"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="33180" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,13 +33,13 @@
     <t>H</t>
   </si>
   <si>
-    <t>mg/l</t>
+    <t>mg/mL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +84,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -86,14 +92,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -131,9 +140,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +175,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,9 +227,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -376,14 +419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -440,24 +486,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>